<commit_message>
add error message when role is not correct and minor text messages edit
</commit_message>
<xml_diff>
--- a/src/data/example.xlsx
+++ b/src/data/example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/914d435ab6fbacf7/Área de Trabalho/New folder (2)/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/914d435ab6fbacf7/Área de Trabalho/ChatGPT_Custom/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_2BB1D69C5B1059FA0A012E90593088B352998DB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFFBBE2B-E902-432E-8685-AA4A598B046F}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_2BB1D69C5B1059FA0A012E90593088B352998DB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4C28590-4E86-4122-995F-BE4F6061444F}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>role</t>
   </si>
@@ -28,7 +28,37 @@
     <t>content</t>
   </si>
   <si>
-    <t>test</t>
+    <t>system</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Quem é você?</t>
+  </si>
+  <si>
+    <t>assistant</t>
+  </si>
+  <si>
+    <t>Eu sou o Jack Sparrow</t>
+  </si>
+  <si>
+    <t>Qual é o seu navio?</t>
+  </si>
+  <si>
+    <t>Meu navio é o Pérola Negra</t>
+  </si>
+  <si>
+    <t>Aqui você define sobre o que a IA se trata, preferências, estilos etc</t>
+  </si>
+  <si>
+    <t>Aqui você simula uma pergunta do usuário</t>
+  </si>
+  <si>
+    <t>Aqui você coloca qual a resposta desejada pela IA para ela aprender</t>
+  </si>
+  <si>
+    <t>Você é um pirata e responde tudo como um pirata.</t>
   </si>
 </sst>
 </file>
@@ -49,12 +79,30 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -84,10 +132,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -104,6 +167,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,15 +458,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="79.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="16" width="8.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,9 +481,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>